<commit_message>
Fixed BOM Crystal Labels
Pointed out by forum user “christine_le”.
</commit_message>
<xml_diff>
--- a/BLEduino/BOM/BOM.xlsx
+++ b/BLEduino/BOM/BOM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Github\bleduino-hardware\BLEduino\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="6705" tabRatio="500"/>
+    <workbookView xWindow="3520" yWindow="1760" windowWidth="21500" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BLEduinoShieldShield 20140717" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BLEduinoShieldShield 20140717'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -330,9 +325,6 @@
     <t>CTX732CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Y2, Y3, Y4 </t>
-  </si>
-  <si>
     <t>Crystal 32,768KHz</t>
   </si>
   <si>
@@ -859,15 +851,18 @@
       <t>-&gt;IPTG23K-Q-T/R</t>
     </r>
   </si>
+  <si>
+    <t>X1, X3, X4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;NT$&quot;* #,##0_ ;_-&quot;NT$&quot;* \-#,##0\ ;_-&quot;NT$&quot;* &quot;-&quot;_ ;_-@_ "/>
-    <numFmt numFmtId="165" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;NT$&quot;* #,##0_ ;_-&quot;NT$&quot;* \-#,##0\ ;_-&quot;NT$&quot;* &quot;-&quot;_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1042,7 +1037,7 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1088,10 +1083,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1518,40 +1513,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.5" style="3" customWidth="1"/>
     <col min="12" max="12" width="19" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14.625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="3" customWidth="1"/>
     <col min="14" max="14" width="9" style="3" customWidth="1"/>
     <col min="15" max="15" width="12.5" style="3" customWidth="1"/>
-    <col min="16" max="16" width="13.125" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="3"/>
+    <col min="16" max="16" width="13.1640625" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="18" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="18" customFormat="1" ht="39" customHeight="1">
       <c r="A1" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>0</v>
@@ -1592,10 +1587,10 @@
       <c r="R1" s="17"/>
       <c r="S1" s="17"/>
     </row>
-    <row r="2" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="39" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1615,7 +1610,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="18">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -1656,7 +1651,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
     </row>
-    <row r="4" spans="1:19" s="14" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="14" customFormat="1" ht="36">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -1694,7 +1689,7 @@
       <c r="M4" s="12"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -1729,7 +1724,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A6" s="29">
         <v>4</v>
       </c>
@@ -1764,7 +1759,7 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
     </row>
-    <row r="7" spans="1:19" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="10" customFormat="1" ht="18">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -1805,7 +1800,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="1:19" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="10" customFormat="1" ht="18">
       <c r="A8" s="29">
         <v>6</v>
       </c>
@@ -1846,7 +1841,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:19" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="10" customFormat="1" ht="18">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -1887,7 +1882,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:19" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="10" customFormat="1" ht="36">
       <c r="A10" s="29">
         <v>8</v>
       </c>
@@ -1928,7 +1923,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:19" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="15" customFormat="1" ht="36">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -1969,7 +1964,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
     </row>
-    <row r="12" spans="1:19" s="15" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="15" customFormat="1" ht="54">
       <c r="A12" s="29">
         <v>10</v>
       </c>
@@ -1980,7 +1975,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>59</v>
@@ -2006,7 +2001,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -2017,7 +2012,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>59</v>
@@ -2043,7 +2038,7 @@
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
     </row>
-    <row r="14" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A14" s="29">
         <v>12</v>
       </c>
@@ -2054,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>59</v>
@@ -2080,7 +2075,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -2091,7 +2086,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>59</v>
@@ -2117,7 +2112,7 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
     </row>
-    <row r="16" spans="1:19" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="15" customFormat="1" ht="18">
       <c r="A16" s="29">
         <v>14</v>
       </c>
@@ -2128,7 +2123,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>32</v>
@@ -2154,7 +2149,7 @@
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
     </row>
-    <row r="17" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -2165,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>59</v>
@@ -2191,7 +2186,7 @@
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
     </row>
-    <row r="18" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A18" s="29">
         <v>16</v>
       </c>
@@ -2202,7 +2197,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>59</v>
@@ -2228,7 +2223,7 @@
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
     </row>
-    <row r="19" spans="1:17" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="15" customFormat="1" ht="36">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -2239,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>81</v>
@@ -2265,7 +2260,7 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
     </row>
-    <row r="20" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A20" s="29">
         <v>18</v>
       </c>
@@ -2276,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E20" s="31" t="s">
         <v>59</v>
@@ -2302,7 +2297,7 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
     </row>
-    <row r="21" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A21" s="21">
         <v>19</v>
       </c>
@@ -2313,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>59</v>
@@ -2337,7 +2332,7 @@
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
     </row>
-    <row r="22" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A22" s="29">
         <v>20</v>
       </c>
@@ -2348,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E22" s="31" t="s">
         <v>32</v>
@@ -2374,7 +2369,7 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
     </row>
-    <row r="23" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A23" s="21">
         <v>21</v>
       </c>
@@ -2413,7 +2408,7 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
     </row>
-    <row r="24" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="10" customFormat="1" ht="32">
       <c r="A24" s="29">
         <v>22</v>
       </c>
@@ -2441,7 +2436,7 @@
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="32" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="L24" s="11"/>
       <c r="M24" s="12"/>
@@ -2450,21 +2445,21 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A25" s="21">
         <v>23</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="21">
         <v>1</v>
       </c>
       <c r="D25" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="F25" s="21">
         <v>2</v>
@@ -2474,11 +2469,11 @@
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J25" s="21"/>
       <c r="K25" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L25" s="11"/>
       <c r="M25" s="12"/>
@@ -2487,21 +2482,21 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
     </row>
-    <row r="26" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A26" s="29">
         <v>24</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="29">
         <v>1</v>
       </c>
       <c r="D26" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="31" t="s">
         <v>107</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>108</v>
       </c>
       <c r="F26" s="29">
         <v>2</v>
@@ -2511,11 +2506,11 @@
       </c>
       <c r="H26" s="29"/>
       <c r="I26" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J26" s="29"/>
       <c r="K26" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L26" s="11"/>
       <c r="M26" s="12"/>
@@ -2524,21 +2519,21 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
     </row>
-    <row r="27" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A27" s="21">
         <v>25</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27" s="21">
         <v>1</v>
       </c>
       <c r="D27" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>112</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>113</v>
       </c>
       <c r="F27" s="21">
         <v>2</v>
@@ -2548,11 +2543,11 @@
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J27" s="21"/>
       <c r="K27" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="12"/>
@@ -2561,18 +2556,18 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
     </row>
-    <row r="28" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A28" s="29">
         <v>26</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C28" s="29">
         <v>1</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E28" s="31" t="s">
         <v>32</v>
@@ -2585,11 +2580,11 @@
       </c>
       <c r="H28" s="29"/>
       <c r="I28" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J28" s="29"/>
       <c r="K28" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="12"/>
@@ -2598,18 +2593,18 @@
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
     </row>
-    <row r="29" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A29" s="21">
         <v>27</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" s="21">
         <v>1</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>32</v>
@@ -2622,7 +2617,7 @@
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="24" t="s">
@@ -2635,18 +2630,18 @@
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
     </row>
-    <row r="30" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A30" s="29">
         <v>28</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="29">
         <v>3</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>32</v>
@@ -2659,11 +2654,11 @@
       </c>
       <c r="H30" s="29"/>
       <c r="I30" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="12"/>
@@ -2672,18 +2667,18 @@
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
     </row>
-    <row r="31" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A31" s="21">
         <v>29</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="21">
         <v>3</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>12</v>
@@ -2695,16 +2690,16 @@
         <v>13</v>
       </c>
       <c r="H31" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="I31" s="21" t="s">
+      <c r="J31" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="K31" s="24" t="s">
         <v>127</v>
-      </c>
-      <c r="J31" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="K31" s="24" t="s">
-        <v>128</v>
       </c>
       <c r="L31" s="11"/>
       <c r="M31" s="12"/>
@@ -2713,18 +2708,18 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
     </row>
-    <row r="32" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A32" s="29">
         <v>30</v>
       </c>
       <c r="B32" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="29">
+        <v>2</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="C32" s="29">
-        <v>2</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>130</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>12</v>
@@ -2736,16 +2731,16 @@
         <v>13</v>
       </c>
       <c r="H32" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="I32" s="29" t="s">
+      <c r="J32" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K32" s="32" t="s">
         <v>132</v>
-      </c>
-      <c r="J32" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>133</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="12"/>
@@ -2754,18 +2749,18 @@
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
     </row>
-    <row r="33" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A33" s="21">
         <v>31</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C33" s="21">
         <v>1</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>81</v>
@@ -2778,11 +2773,11 @@
       </c>
       <c r="H33" s="21"/>
       <c r="I33" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J33" s="21"/>
       <c r="K33" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="12"/>
@@ -2791,18 +2786,18 @@
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
     </row>
-    <row r="34" spans="1:17" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="10" customFormat="1" ht="54">
       <c r="A34" s="29">
         <v>32</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C34" s="29">
         <v>12</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E34" s="31" t="s">
         <v>59</v>
@@ -2815,11 +2810,11 @@
       </c>
       <c r="H34" s="29"/>
       <c r="I34" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J34" s="29"/>
       <c r="K34" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="12"/>
@@ -2828,18 +2823,18 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
     </row>
-    <row r="35" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A35" s="21">
         <v>33</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C35" s="37">
         <v>4</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>59</v>
@@ -2852,11 +2847,11 @@
       </c>
       <c r="H35" s="21"/>
       <c r="I35" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J35" s="21"/>
       <c r="K35" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="12"/>
@@ -2865,18 +2860,18 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
     </row>
-    <row r="36" spans="1:17" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="15" customFormat="1" ht="18">
       <c r="A36" s="29">
         <v>34</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="29">
         <v>1</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="29"/>
@@ -2885,7 +2880,7 @@
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
       <c r="K36" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="12"/>
@@ -2894,18 +2889,18 @@
       <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
     </row>
-    <row r="37" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A37" s="21">
         <v>35</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" s="21">
         <v>2</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>59</v>
@@ -2918,11 +2913,11 @@
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="12"/>
@@ -2931,18 +2926,18 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A38" s="29">
         <v>36</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C38" s="29">
         <v>2</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E38" s="31" t="s">
         <v>59</v>
@@ -2955,11 +2950,11 @@
       </c>
       <c r="H38" s="29"/>
       <c r="I38" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J38" s="29"/>
       <c r="K38" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L38" s="11"/>
       <c r="M38" s="12"/>
@@ -2968,18 +2963,18 @@
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A39" s="21">
         <v>37</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="21">
         <v>1</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E39" s="23" t="s">
         <v>59</v>
@@ -2992,11 +2987,11 @@
       </c>
       <c r="H39" s="21"/>
       <c r="I39" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J39" s="21"/>
       <c r="K39" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L39" s="11"/>
       <c r="M39" s="12"/>
@@ -3005,18 +3000,18 @@
       <c r="P39" s="9"/>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40" spans="1:17" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="10" customFormat="1" ht="18">
       <c r="A40" s="29">
         <v>38</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" s="29">
         <v>1</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E40" s="31" t="s">
         <v>59</v>
@@ -3031,7 +3026,7 @@
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
       <c r="K40" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L40" s="11"/>
       <c r="M40" s="12"/>
@@ -3040,21 +3035,21 @@
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
     </row>
-    <row r="41" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A41" s="21">
         <v>39</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" s="21">
         <v>1</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F41" s="21">
         <v>4</v>
@@ -3064,11 +3059,11 @@
       </c>
       <c r="H41" s="21"/>
       <c r="I41" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J41" s="21"/>
       <c r="K41" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L41" s="11"/>
       <c r="M41" s="12"/>
@@ -3077,37 +3072,37 @@
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
     </row>
-    <row r="42" spans="1:17" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="10" customFormat="1" ht="54">
       <c r="A42" s="29">
         <v>40</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C42" s="29">
         <v>1</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E42" s="31"/>
       <c r="F42" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="G42" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="G42" s="29" t="s">
+      <c r="H42" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="H42" s="29" t="s">
+      <c r="I42" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="I42" s="29" t="s">
+      <c r="J42" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42" s="32" t="s">
         <v>166</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="K42" s="32" t="s">
-        <v>167</v>
       </c>
       <c r="L42" s="11"/>
       <c r="M42" s="12"/>
@@ -3116,12 +3111,12 @@
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
     </row>
-    <row r="43" spans="1:17" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" s="10" customFormat="1" ht="36">
       <c r="A43" s="21">
         <v>41</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C43" s="21">
         <v>1</v>
@@ -3132,7 +3127,7 @@
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
       <c r="I43" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J43" s="22"/>
       <c r="K43" s="24"/>
@@ -3143,7 +3138,7 @@
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
     </row>
-    <row r="44" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="18">
       <c r="A44" s="1"/>
       <c r="B44" s="7"/>
       <c r="C44" s="1"/>
@@ -3153,7 +3148,7 @@
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="7"/>
       <c r="C45" s="1"/>
@@ -3163,11 +3158,11 @@
       <c r="O45" s="8"/>
       <c r="P45" s="8"/>
     </row>
-    <row r="46" spans="1:17" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:17" ht="13" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="46" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -3182,7 +3177,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>